<commit_message>
2/6/17 Capture of work hours time sheets.  These are UnSubmitted but ready
</commit_message>
<xml_diff>
--- a/workHours/Delta_DiligenteTech/1_23_17-1_29_17 Diligente- Weekly TimeSheetMA.xlsx
+++ b/workHours/Delta_DiligenteTech/1_23_17-1_29_17 Diligente- Weekly TimeSheetMA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20430" windowHeight="8970"/>
+    <workbookView xWindow="0" yWindow="1830" windowWidth="20430" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Time Sheet" sheetId="1" r:id="rId1"/>
@@ -611,27 +611,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -640,6 +623,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -659,6 +645,20 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,6 +785,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6353175" cy="6353175"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1089,7 +1137,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="F20" sqref="F20:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1138,19 +1186,19 @@
     </row>
     <row r="2" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5"/>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="49" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="50"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -1211,10 +1259,10 @@
         <v>4</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="51"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -1234,21 +1282,21 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="8"/>
       <c r="G5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="52" t="s">
+      <c r="I5" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="53"/>
+      <c r="J5" s="47"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -1268,21 +1316,21 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
       <c r="F6" s="8"/>
       <c r="G6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="53"/>
+      <c r="J6" s="47"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -1311,10 +1359,10 @@
         <v>11</v>
       </c>
       <c r="H7" s="6"/>
-      <c r="I7" s="55" t="s">
+      <c r="I7" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="53"/>
+      <c r="J7" s="47"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -1396,10 +1444,10 @@
     </row>
     <row r="10" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="59"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="39"/>
       <c r="E10" s="14" t="s">
         <v>17</v>
@@ -1410,7 +1458,7 @@
       <c r="G10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="38" t="s">
         <v>20</v>
       </c>
       <c r="I10" s="39"/>
@@ -1439,9 +1487,8 @@
       <c r="B11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="38" t="str">
-        <f>IF($D$8=0,"",$D$8-6)</f>
-        <v/>
+      <c r="C11" s="59">
+        <v>42758</v>
       </c>
       <c r="D11" s="39"/>
       <c r="E11" s="19" t="s">
@@ -1453,8 +1500,8 @@
       <c r="G11" s="20">
         <v>8</v>
       </c>
-      <c r="H11" s="44"/>
-      <c r="I11" s="45"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="58"/>
       <c r="J11" s="21">
         <f t="shared" ref="J11:J17" si="0">IF(G11+H11&gt;24,"Total &gt; 24 hours.",SUM(G11,H11))</f>
         <v>8</v>
@@ -1481,9 +1528,8 @@
       <c r="B12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="38" t="str">
-        <f>IF($D$8=0,"",$D$8-5)</f>
-        <v/>
+      <c r="C12" s="59">
+        <v>42759</v>
       </c>
       <c r="D12" s="39"/>
       <c r="E12" s="19" t="s">
@@ -1495,7 +1541,7 @@
       <c r="G12" s="25">
         <v>8</v>
       </c>
-      <c r="H12" s="40"/>
+      <c r="H12" s="56"/>
       <c r="I12" s="39"/>
       <c r="J12" s="26">
         <f t="shared" si="0"/>
@@ -1523,9 +1569,8 @@
       <c r="B13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="38" t="str">
-        <f>IF($D$8=0,"",$D$8-4)</f>
-        <v/>
+      <c r="C13" s="59">
+        <v>42760</v>
       </c>
       <c r="D13" s="39"/>
       <c r="E13" s="19" t="s">
@@ -1537,7 +1582,7 @@
       <c r="G13" s="25">
         <v>8</v>
       </c>
-      <c r="H13" s="40"/>
+      <c r="H13" s="56"/>
       <c r="I13" s="39"/>
       <c r="J13" s="26">
         <f t="shared" si="0"/>
@@ -1565,9 +1610,8 @@
       <c r="B14" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="38" t="str">
-        <f>IF($D$8=0,"",$D$8-3)</f>
-        <v/>
+      <c r="C14" s="59">
+        <v>42761</v>
       </c>
       <c r="D14" s="39"/>
       <c r="E14" s="19" t="s">
@@ -1579,7 +1623,7 @@
       <c r="G14" s="25">
         <v>8</v>
       </c>
-      <c r="H14" s="40"/>
+      <c r="H14" s="56"/>
       <c r="I14" s="39"/>
       <c r="J14" s="26">
         <f t="shared" si="0"/>
@@ -1607,9 +1651,8 @@
       <c r="B15" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="38" t="str">
-        <f>IF($D$8=0,"",$D$8-2)</f>
-        <v/>
+      <c r="C15" s="59">
+        <v>42762</v>
       </c>
       <c r="D15" s="39"/>
       <c r="E15" s="19" t="s">
@@ -1621,7 +1664,7 @@
       <c r="G15" s="25">
         <v>8</v>
       </c>
-      <c r="H15" s="40"/>
+      <c r="H15" s="56"/>
       <c r="I15" s="39"/>
       <c r="J15" s="26">
         <f t="shared" si="0"/>
@@ -1649,7 +1692,7 @@
       <c r="B16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="38" t="str">
+      <c r="C16" s="59" t="str">
         <f>IF($D$8=0,"",$D$8-1)</f>
         <v/>
       </c>
@@ -1657,7 +1700,7 @@
       <c r="E16" s="23"/>
       <c r="F16" s="24"/>
       <c r="G16" s="25"/>
-      <c r="H16" s="40"/>
+      <c r="H16" s="56"/>
       <c r="I16" s="39"/>
       <c r="J16" s="26">
         <f t="shared" si="0"/>
@@ -1685,7 +1728,7 @@
       <c r="B17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="38" t="str">
+      <c r="C17" s="59" t="str">
         <f>IF($D$8=0,"",$D$8)</f>
         <v/>
       </c>
@@ -1693,7 +1736,7 @@
       <c r="E17" s="23"/>
       <c r="F17" s="24"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="40"/>
+      <c r="H17" s="56"/>
       <c r="I17" s="39"/>
       <c r="J17" s="26">
         <f t="shared" si="0"/>
@@ -1729,7 +1772,7 @@
         <f t="shared" ref="G18:H18" si="1">SUM(G11:G17)</f>
         <v>40</v>
       </c>
-      <c r="H18" s="43">
+      <c r="H18" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1789,12 +1832,12 @@
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
-      <c r="F20" s="41" t="s">
+      <c r="F20" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
       <c r="J20" s="31">
         <v>42765</v>
       </c>
@@ -1853,12 +1896,12 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
       <c r="J22" s="31">
         <v>42765</v>
       </c>
@@ -29269,6 +29312,23 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="F20:I20"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
@@ -29279,23 +29339,6 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B10:D10"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>